<commit_message>
done: fix bug with message that have blank space. add doc todo: register feature
</commit_message>
<xml_diff>
--- a/status codes and bugs to fix.xlsx
+++ b/status codes and bugs to fix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Limited\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Limited\IdeaProjects\ApplicationProtocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -96,7 +96,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +125,14 @@
       <charset val="222"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="0.39997558519241921"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="222"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -146,13 +154,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
@@ -517,22 +526,22 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>